<commit_message>
Arreglos Interfaz. Iconos página de inicio, cambio de color a rojo
</commit_message>
<xml_diff>
--- a/fun.xlsx
+++ b/fun.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Ausen2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB1E432-1C8D-4FEF-B4FF-5117743817F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D84C45-ED9C-4DF2-B773-2A7B39C03F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36570" yWindow="-3495" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35265" yWindow="-2190" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcinarios Unicauca 2022" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="105">
   <si>
     <t>CODIGO</t>
   </si>
@@ -99,9 +99,6 @@
     <t>ALEGRIA MARTINEZ VIVIANA</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>FEM</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>8366861-3165460655</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>PROFESOR ASOCIADO</t>
   </si>
   <si>
@@ -325,6 +319,27 @@
   </si>
   <si>
     <t>ANDRES DIAGO</t>
+  </si>
+  <si>
+    <t>ANDRES DIAGO f</t>
+  </si>
+  <si>
+    <t>ANDRES DIAGO g</t>
+  </si>
+  <si>
+    <t>MASc</t>
+  </si>
+  <si>
+    <t>MAS3</t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>ACT23</t>
   </si>
 </sst>
 </file>
@@ -643,17 +658,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="25.33203125" customWidth="1"/>
-    <col min="12" max="12" width="20.21875" customWidth="1"/>
-    <col min="13" max="13" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="25.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.21875" customWidth="1"/>
+    <col min="12" max="12" width="26.109375" customWidth="1"/>
+    <col min="22" max="22" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -670,61 +686,61 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
@@ -735,61 +751,61 @@
         <v>34561628</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1">
         <v>44810</v>
       </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2">
+      <c r="E2">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
-        <v>25</v>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2">
+        <v>7200</v>
       </c>
       <c r="H2">
-        <v>7200</v>
-      </c>
-      <c r="I2">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2">
+        <v>1113003</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
         <v>40</v>
       </c>
-      <c r="K2">
-        <v>1113003</v>
-      </c>
-      <c r="L2" t="s">
-        <v>41</v>
-      </c>
-      <c r="M2" t="s">
-        <v>42</v>
+      <c r="M2">
+        <v>4</v>
       </c>
       <c r="N2">
-        <v>4</v>
-      </c>
-      <c r="O2">
         <v>5608354</v>
       </c>
-      <c r="P2" s="1">
+      <c r="O2" s="1">
         <v>26417</v>
       </c>
-      <c r="Q2">
+      <c r="P2">
         <v>50</v>
       </c>
-      <c r="S2">
+      <c r="R2">
         <v>29</v>
       </c>
+      <c r="T2" t="s">
+        <v>50</v>
+      </c>
       <c r="U2" t="s">
-        <v>52</v>
-      </c>
-      <c r="V2" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2">
+        <v>51</v>
+      </c>
+      <c r="V2">
         <v>8242599</v>
+      </c>
+      <c r="W2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
@@ -800,61 +816,61 @@
         <v>76305479</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1">
         <v>44810</v>
       </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3">
+      <c r="E3">
         <v>40</v>
       </c>
-      <c r="G3" t="s">
-        <v>31</v>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>7200</v>
       </c>
       <c r="H3">
-        <v>7200</v>
-      </c>
-      <c r="I3">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3">
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3">
         <v>1173009</v>
       </c>
+      <c r="K3" t="s">
+        <v>48</v>
+      </c>
       <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
       </c>
       <c r="N3">
-        <v>4</v>
-      </c>
-      <c r="O3">
         <v>5277561</v>
       </c>
-      <c r="P3" s="1">
+      <c r="O3" s="1">
         <v>24596</v>
       </c>
-      <c r="Q3">
+      <c r="P3">
         <v>55</v>
       </c>
-      <c r="S3">
+      <c r="R3">
         <v>29</v>
       </c>
+      <c r="T3" t="s">
+        <v>53</v>
+      </c>
       <c r="U3" t="s">
-        <v>55</v>
-      </c>
-      <c r="V3" t="s">
-        <v>56</v>
-      </c>
-      <c r="W3">
+        <v>54</v>
+      </c>
+      <c r="V3">
         <v>8231768</v>
+      </c>
+      <c r="W3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
@@ -865,61 +881,61 @@
         <v>25270247</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1">
         <v>44810</v>
       </c>
-      <c r="E4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4">
+      <c r="E4">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
-        <v>25</v>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4">
+        <v>7200</v>
       </c>
       <c r="H4">
-        <v>7200</v>
-      </c>
-      <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4">
+        <v>1113001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
         <v>40</v>
       </c>
-      <c r="K4">
-        <v>1113001</v>
-      </c>
-      <c r="L4" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
+      <c r="M4">
+        <v>4</v>
       </c>
       <c r="N4">
-        <v>4</v>
-      </c>
-      <c r="O4">
         <v>4563364</v>
       </c>
-      <c r="P4" s="1">
+      <c r="O4" s="1">
         <v>18295</v>
       </c>
-      <c r="Q4">
+      <c r="P4">
         <v>72</v>
       </c>
-      <c r="S4">
+      <c r="R4">
         <v>29</v>
       </c>
+      <c r="T4" t="s">
+        <v>56</v>
+      </c>
       <c r="U4" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" t="s">
-        <v>59</v>
-      </c>
-      <c r="W4">
+        <v>57</v>
+      </c>
+      <c r="V4">
         <v>8244669</v>
+      </c>
+      <c r="W4" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
@@ -935,56 +951,56 @@
       <c r="D5" s="1">
         <v>39918</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="F5">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>2044</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
         <v>25</v>
       </c>
-      <c r="H5">
-        <v>2044</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="J5">
+        <v>1029001</v>
+      </c>
+      <c r="K5" t="s">
         <v>26</v>
       </c>
-      <c r="K5">
-        <v>1029001</v>
-      </c>
       <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>2607609</v>
+      </c>
+      <c r="O5" s="1">
+        <v>30578</v>
+      </c>
+      <c r="P5">
+        <v>39</v>
+      </c>
+      <c r="R5">
+        <v>14</v>
+      </c>
+      <c r="T5" t="s">
         <v>27</v>
-      </c>
-      <c r="M5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>2607609</v>
-      </c>
-      <c r="P5" s="1">
-        <v>30578</v>
-      </c>
-      <c r="Q5">
-        <v>39</v>
-      </c>
-      <c r="S5">
-        <v>14</v>
       </c>
       <c r="U5" t="s">
         <v>28</v>
       </c>
-      <c r="V5" t="s">
-        <v>29</v>
-      </c>
-      <c r="W5">
+      <c r="V5">
         <v>8278946</v>
+      </c>
+      <c r="W5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -995,61 +1011,61 @@
         <v>10548083</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1">
         <v>44810</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>7200</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6">
+        <v>1143006</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
         <v>37</v>
       </c>
-      <c r="F6">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6">
-        <v>7200</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6">
-        <v>1143006</v>
-      </c>
-      <c r="L6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" t="s">
-        <v>39</v>
+      <c r="M6">
+        <v>4</v>
       </c>
       <c r="N6">
-        <v>4</v>
-      </c>
-      <c r="O6">
         <v>2609844</v>
       </c>
-      <c r="P6" s="1">
+      <c r="O6" s="1">
         <v>23906</v>
       </c>
-      <c r="Q6">
+      <c r="P6">
         <v>57</v>
       </c>
-      <c r="S6">
+      <c r="R6">
         <v>29</v>
       </c>
+      <c r="T6" t="s">
+        <v>59</v>
+      </c>
       <c r="U6" t="s">
+        <v>60</v>
+      </c>
+      <c r="V6" t="s">
         <v>61</v>
       </c>
-      <c r="V6" t="s">
-        <v>62</v>
-      </c>
       <c r="W6" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -1060,61 +1076,61 @@
         <v>76306673</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D7" s="1">
         <v>44823</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>8300</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7">
+        <v>1143006</v>
+      </c>
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
         <v>37</v>
       </c>
-      <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7">
-        <v>8300</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>2630560</v>
+      </c>
+      <c r="O7" s="1">
+        <v>24875</v>
+      </c>
+      <c r="P7">
+        <v>54</v>
+      </c>
+      <c r="R7">
+        <v>30</v>
+      </c>
+      <c r="T7" t="s">
+        <v>64</v>
+      </c>
+      <c r="U7" t="s">
         <v>65</v>
       </c>
-      <c r="K7">
-        <v>1143006</v>
-      </c>
-      <c r="L7" t="s">
-        <v>44</v>
-      </c>
-      <c r="M7" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7">
-        <v>5</v>
-      </c>
-      <c r="O7">
-        <v>2630560</v>
-      </c>
-      <c r="P7" s="1">
-        <v>24875</v>
-      </c>
-      <c r="Q7">
-        <v>54</v>
-      </c>
-      <c r="S7">
-        <v>30</v>
-      </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>66</v>
       </c>
-      <c r="V7" t="s">
-        <v>67</v>
-      </c>
       <c r="W7" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -1125,61 +1141,61 @@
         <v>34559165</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1">
         <v>44810</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8">
+        <v>7200</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8">
+        <v>1143011</v>
+      </c>
+      <c r="K8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" t="s">
         <v>37</v>
       </c>
-      <c r="F8">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8">
-        <v>7200</v>
-      </c>
-      <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8">
-        <v>1143011</v>
-      </c>
-      <c r="L8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" t="s">
-        <v>39</v>
+      <c r="M8">
+        <v>4</v>
       </c>
       <c r="N8">
-        <v>4</v>
-      </c>
-      <c r="O8">
         <v>2803191</v>
       </c>
-      <c r="P8" s="1">
+      <c r="O8" s="1">
         <v>26126</v>
       </c>
-      <c r="Q8">
+      <c r="P8">
         <v>51</v>
       </c>
-      <c r="S8">
+      <c r="R8">
         <v>29</v>
       </c>
+      <c r="T8" t="s">
+        <v>68</v>
+      </c>
       <c r="U8" t="s">
-        <v>70</v>
-      </c>
-      <c r="V8" t="s">
-        <v>71</v>
-      </c>
-      <c r="W8">
+        <v>69</v>
+      </c>
+      <c r="V8">
         <v>8364419</v>
+      </c>
+      <c r="W8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -1190,61 +1206,61 @@
         <v>34563785</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="1">
         <v>44810</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9">
+        <v>7200</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9">
+        <v>1143011</v>
+      </c>
+      <c r="K9" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" t="s">
         <v>37</v>
       </c>
-      <c r="F9">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9">
-        <v>7200</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9">
-        <v>1143011</v>
-      </c>
-      <c r="L9" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" t="s">
-        <v>39</v>
+      <c r="M9">
+        <v>4</v>
       </c>
       <c r="N9">
-        <v>4</v>
-      </c>
-      <c r="O9">
         <v>2474371</v>
       </c>
-      <c r="P9" s="1">
+      <c r="O9" s="1">
         <v>26814</v>
       </c>
-      <c r="Q9">
+      <c r="P9">
         <v>49</v>
       </c>
-      <c r="S9">
+      <c r="R9">
         <v>29</v>
       </c>
+      <c r="T9" t="s">
+        <v>71</v>
+      </c>
       <c r="U9" t="s">
-        <v>73</v>
-      </c>
-      <c r="V9" t="s">
-        <v>74</v>
-      </c>
-      <c r="W9">
+        <v>72</v>
+      </c>
+      <c r="V9">
         <v>8230953</v>
+      </c>
+      <c r="W9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.3">
@@ -1255,52 +1271,52 @@
         <v>76319254</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1">
         <v>42745</v>
       </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10">
+      <c r="E10">
         <v>8</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>4044</v>
+      </c>
+      <c r="H10">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
         <v>31</v>
       </c>
-      <c r="H10">
-        <v>4044</v>
-      </c>
-      <c r="I10">
-        <v>13</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="J10">
+        <v>1042001</v>
+      </c>
+      <c r="K10" t="s">
         <v>32</v>
       </c>
-      <c r="K10">
-        <v>1042001</v>
-      </c>
       <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>1665038</v>
+      </c>
+      <c r="O10" s="1">
+        <v>27098</v>
+      </c>
+      <c r="P10">
+        <v>48</v>
+      </c>
+      <c r="R10">
+        <v>14</v>
+      </c>
+      <c r="T10" t="s">
         <v>33</v>
-      </c>
-      <c r="M10" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10">
-        <v>2</v>
-      </c>
-      <c r="O10">
-        <v>1665038</v>
-      </c>
-      <c r="P10" s="1">
-        <v>27098</v>
-      </c>
-      <c r="Q10">
-        <v>48</v>
-      </c>
-      <c r="S10">
-        <v>14</v>
       </c>
       <c r="U10" t="s">
         <v>34</v>
@@ -1309,7 +1325,7 @@
         <v>35</v>
       </c>
       <c r="W10" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -1320,61 +1336,61 @@
         <v>34511528</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="1">
         <v>44810</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11">
+        <v>7300</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>36</v>
+      </c>
+      <c r="J11">
+        <v>1143012</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" t="s">
         <v>37</v>
       </c>
-      <c r="F11">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11">
-        <v>7300</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11">
-        <v>1143012</v>
-      </c>
-      <c r="L11" t="s">
-        <v>49</v>
-      </c>
-      <c r="M11" t="s">
-        <v>39</v>
+      <c r="M11">
+        <v>4</v>
       </c>
       <c r="N11">
-        <v>4</v>
-      </c>
-      <c r="O11">
         <v>2904796</v>
       </c>
-      <c r="P11" s="1">
+      <c r="O11" s="1">
         <v>23672</v>
       </c>
-      <c r="Q11">
+      <c r="P11">
         <v>57</v>
       </c>
-      <c r="S11">
+      <c r="R11">
         <v>29</v>
       </c>
+      <c r="T11" t="s">
+        <v>74</v>
+      </c>
       <c r="U11" t="s">
+        <v>75</v>
+      </c>
+      <c r="V11" t="s">
         <v>76</v>
       </c>
-      <c r="V11" t="s">
-        <v>77</v>
-      </c>
       <c r="W11" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.3">
@@ -1385,61 +1401,61 @@
         <v>34533885</v>
       </c>
       <c r="C12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D12" s="1">
         <v>44810</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12">
+        <v>7200</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12">
+        <v>1143012</v>
+      </c>
+      <c r="K12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" t="s">
         <v>37</v>
       </c>
-      <c r="F12">
-        <v>40</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12">
-        <v>7200</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12">
-        <v>1143012</v>
-      </c>
-      <c r="L12" t="s">
-        <v>49</v>
-      </c>
-      <c r="M12" t="s">
-        <v>39</v>
+      <c r="M12">
+        <v>4</v>
       </c>
       <c r="N12">
-        <v>4</v>
-      </c>
-      <c r="O12">
         <v>4948741</v>
       </c>
-      <c r="P12" s="1">
+      <c r="O12" s="1">
         <v>20819</v>
       </c>
-      <c r="Q12">
+      <c r="P12">
         <v>65</v>
       </c>
-      <c r="S12">
+      <c r="R12">
         <v>29</v>
       </c>
+      <c r="T12" t="s">
+        <v>78</v>
+      </c>
       <c r="U12" t="s">
-        <v>80</v>
-      </c>
-      <c r="V12" t="s">
-        <v>81</v>
-      </c>
-      <c r="W12">
+        <v>79</v>
+      </c>
+      <c r="V12">
         <v>8244178</v>
+      </c>
+      <c r="W12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
@@ -1450,61 +1466,61 @@
         <v>34552993</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" s="1">
         <v>44810</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13">
+        <v>7300</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13">
+        <v>1143012</v>
+      </c>
+      <c r="K13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L13" t="s">
         <v>37</v>
       </c>
-      <c r="F13">
-        <v>40</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13">
-        <v>7300</v>
-      </c>
-      <c r="I13">
-        <v>3</v>
-      </c>
-      <c r="J13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13">
-        <v>1143012</v>
-      </c>
-      <c r="L13" t="s">
-        <v>49</v>
-      </c>
-      <c r="M13" t="s">
-        <v>39</v>
+      <c r="M13">
+        <v>4</v>
       </c>
       <c r="N13">
-        <v>4</v>
-      </c>
-      <c r="O13">
         <v>6575414</v>
       </c>
-      <c r="P13" s="1">
+      <c r="O13" s="1">
         <v>24948</v>
       </c>
-      <c r="Q13">
+      <c r="P13">
         <v>54</v>
       </c>
-      <c r="S13">
+      <c r="R13">
         <v>29</v>
       </c>
+      <c r="T13" t="s">
+        <v>81</v>
+      </c>
       <c r="U13" t="s">
-        <v>83</v>
-      </c>
-      <c r="V13" t="s">
-        <v>84</v>
-      </c>
-      <c r="W13">
+        <v>82</v>
+      </c>
+      <c r="V13">
         <v>3017310897</v>
+      </c>
+      <c r="W13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
@@ -1515,61 +1531,61 @@
         <v>25517745</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D14" s="1">
         <v>44810</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14">
+        <v>7200</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14">
+        <v>1143012</v>
+      </c>
+      <c r="K14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" t="s">
         <v>37</v>
       </c>
-      <c r="F14">
-        <v>40</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14">
-        <v>7200</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14">
-        <v>1143012</v>
-      </c>
-      <c r="L14" t="s">
-        <v>49</v>
-      </c>
-      <c r="M14" t="s">
-        <v>39</v>
+      <c r="M14">
+        <v>4</v>
       </c>
       <c r="N14">
-        <v>4</v>
-      </c>
-      <c r="O14">
         <v>5606381</v>
       </c>
-      <c r="P14" s="1">
+      <c r="O14" s="1">
         <v>25320</v>
       </c>
-      <c r="Q14">
+      <c r="P14">
         <v>53</v>
       </c>
-      <c r="S14">
+      <c r="R14">
         <v>29</v>
       </c>
+      <c r="T14" t="s">
+        <v>84</v>
+      </c>
       <c r="U14" t="s">
+        <v>85</v>
+      </c>
+      <c r="V14" t="s">
         <v>86</v>
       </c>
-      <c r="V14" t="s">
-        <v>87</v>
-      </c>
       <c r="W14" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
@@ -1580,61 +1596,61 @@
         <v>34551642</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D15" s="1">
         <v>44823</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>8400</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15">
+        <v>1143012</v>
+      </c>
+      <c r="K15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" t="s">
         <v>37</v>
       </c>
-      <c r="F15">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15">
-        <v>8400</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="M15">
+        <v>5</v>
+      </c>
+      <c r="N15">
+        <v>3156672</v>
+      </c>
+      <c r="O15" s="1">
+        <v>24742</v>
+      </c>
+      <c r="P15">
+        <v>55</v>
+      </c>
+      <c r="R15">
+        <v>30</v>
+      </c>
+      <c r="T15" t="s">
+        <v>89</v>
+      </c>
+      <c r="U15" t="s">
         <v>90</v>
       </c>
-      <c r="K15">
-        <v>1143012</v>
-      </c>
-      <c r="L15" t="s">
-        <v>49</v>
-      </c>
-      <c r="M15" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15">
-        <v>5</v>
-      </c>
-      <c r="O15">
-        <v>3156672</v>
-      </c>
-      <c r="P15" s="1">
-        <v>24742</v>
-      </c>
-      <c r="Q15">
-        <v>55</v>
-      </c>
-      <c r="S15">
-        <v>30</v>
-      </c>
-      <c r="U15" t="s">
-        <v>91</v>
-      </c>
-      <c r="V15" t="s">
-        <v>92</v>
-      </c>
-      <c r="W15">
+      <c r="V15">
         <v>8382114</v>
+      </c>
+      <c r="W15" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
@@ -1645,61 +1661,61 @@
         <v>30720867</v>
       </c>
       <c r="C16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D16" s="1">
         <v>44810</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16">
+        <v>7300</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16">
+        <v>1143004</v>
+      </c>
+      <c r="K16" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" t="s">
         <v>37</v>
       </c>
-      <c r="F16">
-        <v>40</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16">
-        <v>7300</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16" t="s">
-        <v>38</v>
-      </c>
-      <c r="K16">
-        <v>1143004</v>
-      </c>
-      <c r="L16" t="s">
-        <v>47</v>
-      </c>
-      <c r="M16" t="s">
-        <v>39</v>
+      <c r="M16">
+        <v>4</v>
       </c>
       <c r="N16">
-        <v>4</v>
-      </c>
-      <c r="O16">
         <v>6329785</v>
       </c>
-      <c r="P16" s="1">
+      <c r="O16" s="1">
         <v>21916</v>
       </c>
-      <c r="Q16">
+      <c r="P16">
         <v>62</v>
       </c>
-      <c r="S16">
+      <c r="R16">
         <v>29</v>
       </c>
+      <c r="T16" t="s">
+        <v>92</v>
+      </c>
       <c r="U16" t="s">
-        <v>94</v>
-      </c>
-      <c r="V16" t="s">
-        <v>95</v>
-      </c>
-      <c r="W16">
+        <v>93</v>
+      </c>
+      <c r="V16">
         <v>8235450</v>
+      </c>
+      <c r="W16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.3">
@@ -1710,61 +1726,61 @@
         <v>34540781</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D17" s="1">
         <v>44810</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17">
+        <v>7200</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17">
+        <v>1143008</v>
+      </c>
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" t="s">
         <v>37</v>
       </c>
-      <c r="F17">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17">
-        <v>7200</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="J17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K17">
-        <v>1143008</v>
-      </c>
-      <c r="L17" t="s">
-        <v>46</v>
-      </c>
-      <c r="M17" t="s">
-        <v>39</v>
+      <c r="M17">
+        <v>4</v>
       </c>
       <c r="N17">
-        <v>4</v>
-      </c>
-      <c r="O17">
         <v>5606381</v>
       </c>
-      <c r="P17" s="1">
+      <c r="O17" s="1">
         <v>23114</v>
       </c>
-      <c r="Q17">
+      <c r="P17">
         <v>59</v>
       </c>
-      <c r="S17">
+      <c r="R17">
         <v>29</v>
       </c>
+      <c r="T17" t="s">
+        <v>95</v>
+      </c>
       <c r="U17" t="s">
-        <v>97</v>
-      </c>
-      <c r="V17" t="s">
-        <v>98</v>
-      </c>
-      <c r="W17">
+        <v>96</v>
+      </c>
+      <c r="V17">
         <v>8316144</v>
+      </c>
+      <c r="W17" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
@@ -1775,61 +1791,191 @@
         <v>1001086246</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1">
         <v>44810</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>7200</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18">
+        <v>1143008</v>
+      </c>
+      <c r="K18" t="s">
+        <v>44</v>
+      </c>
+      <c r="L18" t="s">
         <v>37</v>
       </c>
-      <c r="F18">
+      <c r="M18">
+        <v>4</v>
+      </c>
+      <c r="N18">
+        <v>5006381</v>
+      </c>
+      <c r="O18" s="1">
+        <v>23114</v>
+      </c>
+      <c r="P18">
+        <v>59</v>
+      </c>
+      <c r="R18">
+        <v>29</v>
+      </c>
+      <c r="T18" t="s">
+        <v>95</v>
+      </c>
+      <c r="U18" t="s">
+        <v>96</v>
+      </c>
+      <c r="V18">
+        <v>8316144</v>
+      </c>
+      <c r="W18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20">
+        <v>1001086247</v>
+      </c>
+      <c r="C20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="1">
+        <v>44810</v>
+      </c>
+      <c r="E20">
         <v>40</v>
       </c>
-      <c r="G18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18">
+      <c r="F20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20">
         <v>7200</v>
       </c>
-      <c r="I18">
+      <c r="H20">
         <v>1</v>
       </c>
-      <c r="J18" t="s">
+      <c r="I20" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20">
+        <v>1143008</v>
+      </c>
+      <c r="K20" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+      <c r="N20">
+        <v>5006381</v>
+      </c>
+      <c r="O20" s="1">
+        <v>23114</v>
+      </c>
+      <c r="P20">
+        <v>59</v>
+      </c>
+      <c r="R20">
+        <v>29</v>
+      </c>
+      <c r="T20" t="s">
+        <v>95</v>
+      </c>
+      <c r="U20" t="s">
+        <v>96</v>
+      </c>
+      <c r="V20">
+        <v>8316144</v>
+      </c>
+      <c r="W20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>1001086248</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="1">
+        <v>44810</v>
+      </c>
+      <c r="E21">
         <v>40</v>
       </c>
-      <c r="K18">
+      <c r="F21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21">
+        <v>7200</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21">
         <v>1143008</v>
       </c>
-      <c r="L18" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" t="s">
-        <v>39</v>
-      </c>
-      <c r="N18">
+      <c r="K21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21">
         <v>4</v>
       </c>
-      <c r="O18">
-        <v>5606381</v>
-      </c>
-      <c r="P18" s="1">
+      <c r="N21">
+        <v>5006381</v>
+      </c>
+      <c r="O21" s="1">
         <v>23114</v>
       </c>
-      <c r="Q18">
+      <c r="P21">
         <v>59</v>
       </c>
-      <c r="S18">
+      <c r="R21">
         <v>29</v>
       </c>
-      <c r="U18" t="s">
-        <v>97</v>
-      </c>
-      <c r="V18" t="s">
-        <v>98</v>
-      </c>
-      <c r="W18">
+      <c r="T21" t="s">
+        <v>95</v>
+      </c>
+      <c r="U21" t="s">
+        <v>96</v>
+      </c>
+      <c r="V21">
         <v>8316144</v>
+      </c>
+      <c r="W21" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Terminado filtros tabal consulta. Cargar Funcionario con tabal Auxiliar. Base MySQL ausentismos_v2.sql.
</commit_message>
<xml_diff>
--- a/fun.xlsx
+++ b/fun.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Ausen2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D84C45-ED9C-4DF2-B773-2A7B39C03F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770F7DDD-EF63-4065-92E5-F1D59A9DF847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35265" yWindow="-2190" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcinarios Unicauca 2022" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="107">
   <si>
     <t>CODIGO</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>ACT23</t>
+  </si>
+  <si>
+    <t>MESSI g</t>
+  </si>
+  <si>
+    <t>DEPTO D</t>
   </si>
 </sst>
 </file>
@@ -658,14 +664,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:W22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="3" max="4" width="18.77734375" customWidth="1"/>
     <col min="9" max="9" width="25.33203125" customWidth="1"/>
     <col min="11" max="11" width="20.21875" customWidth="1"/>
     <col min="12" max="12" width="26.109375" customWidth="1"/>
@@ -1978,6 +1985,71 @@
         <v>104</v>
       </c>
     </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3444</v>
+      </c>
+      <c r="B22">
+        <v>2020055</v>
+      </c>
+      <c r="C22" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44810</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22">
+        <v>7200</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22" t="s">
+        <v>38</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22" t="s">
+        <v>106</v>
+      </c>
+      <c r="L22" t="s">
+        <v>37</v>
+      </c>
+      <c r="M22">
+        <v>4</v>
+      </c>
+      <c r="N22">
+        <v>5006381</v>
+      </c>
+      <c r="O22" s="1">
+        <v>23114</v>
+      </c>
+      <c r="P22">
+        <v>59</v>
+      </c>
+      <c r="R22">
+        <v>29</v>
+      </c>
+      <c r="T22" t="s">
+        <v>95</v>
+      </c>
+      <c r="U22" t="s">
+        <v>96</v>
+      </c>
+      <c r="V22">
+        <v>8316144</v>
+      </c>
+      <c r="W22" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>